<commit_message>
add scripts for Monte Carlo simulations
</commit_message>
<xml_diff>
--- a/scripts/Data/modelv5.xlsx
+++ b/scripts/Data/modelv5.xlsx
@@ -1250,16 +1250,16 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <v>0.005557785432514305</v>
+        <v>0.006080101788452492</v>
       </c>
       <c r="F21">
-        <v>1.434510131207401</v>
+        <v>1.376994173579743</v>
       </c>
       <c r="G21">
-        <v>5.512521157774729E-05</v>
+        <v>3.548110086667569E-05</v>
       </c>
       <c r="H21">
-        <v>2.903518118847876</v>
+        <v>2.687699681754618</v>
       </c>
       <c r="I21">
         <v>1</v>

</xml_diff>